<commit_message>
Finish modifying search string by blocks -- across all the blocks all the test list articles are retreived.
</commit_message>
<xml_diff>
--- a/data/derived-data/screen_test_list/test-list_2023-01-19.xlsx
+++ b/data/derived-data/screen_test_list/test-list_2023-01-19.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -888,12 +888,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Life cycle assessment of carbon dioxide removal technologies: a critical review</t>
+          <t>Current trends and prospects of tidal energy technology</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Terlouw, T and Bauer, C and Rosa, L and Mazzotti, M</t>
+          <t>Chowdhury, MS and Rahman, KS and Selvanathan, V and Nuthammachot, N and Suklueng, M and Mostafaeipour, A and Habib, A and Akhtaruzzaman and Amin, N and Techato, K</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -903,41 +903,41 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>10.1039/d0ee03757e</t>
+          <t>10.1007/s10668-020-01013-4</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Current trends and prospects of tidal energy technology</t>
+          <t>Geoengineering with seagrasses: is credit due where credit is given?</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Chowdhury, MS and Rahman, KS and Selvanathan, V and Nuthammachot, N and Suklueng, M and Mostafaeipour, A and Habib, A and Akhtaruzzaman and Amin, N and Techato, K</t>
+          <t>Johannessen, SC and Macdonald, RW</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>10.1007/s10668-020-01013-4</t>
+          <t>10.1088/1748-9326/11/11/113001</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Geoengineering with seagrasses: is credit due where credit is given?</t>
+          <t>Could artificial ocean alkalinization protect tropical coral ecosystems from ocean acidification?</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Johannessen, SC and Macdonald, RW</t>
+          <t>Feng, EY and Keller, DP and Koeve, W and Oschlies, A</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -947,305 +947,305 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>10.1088/1748-9326/11/11/113001</t>
+          <t>10.1088/1748-9326/11/7/074008</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Could artificial ocean alkalinization protect tropical coral ecosystems from ocean acidification?</t>
+          <t>Analysis of the environmental issues concerning the deployment of an OTEC power plant in Martinique</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Feng, EY and Keller, DP and Koeve, W and Oschlies, A</t>
+          <t>Devault, DA and Pene-Annette, A</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>10.1088/1748-9326/11/7/074008</t>
+          <t>10.1007/s11356-017-8749-3</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Provision of ecosystem services by human-made structures in a highly impacted estuary</t>
+          <t>Benefits of coastal managed realignment for society: Evidence from ecosystem service assessments in two UK regions</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Layman, CA and Jud, ZR and Archer, SK and Riera, D</t>
+          <t>MacDonald, MA and de Ruyck, C and Field, RH and Bedford, A and Bradbury, RB</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>10.1088/1748-9326/9/4/044009</t>
+          <t>10.1016/j.ecss.2017.09.007</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Analysis of the environmental issues concerning the deployment of an OTEC power plant in Martinique</t>
+          <t>Climate change adaptation in fisheries</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Devault, DA and Pene-Annette, A</t>
+          <t>Galappaththi, EK and Susarla, VB and Loutet, SJT and Ichien, ST and Hyman, AA and Ford, JD</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>10.1007/s11356-017-8749-3</t>
+          <t>10.1111/faf.12595</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Benefits of coastal managed realignment for society: Evidence from ecosystem service assessments in two UK regions</t>
+          <t>Resilience and Social Adaptation to Climate Change Impacts in Small-Scale Fisheries</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>MacDonald, MA and de Ruyck, C and Field, RH and Bedford, A and Bradbury, RB</t>
+          <t>Villasante, S and Macho, G and Silva, MRO and Lopes, PFM and Pita, P and Simon, A and Balsa, JCM and Olabarria, C and Vazquez, E and Calvo, N</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>10.1016/j.ecss.2017.09.007</t>
+          <t>10.3389/fmars.2022.802762</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Climate change adaptation in fisheries</t>
+          <t>Responding to Climate Change: Participatory Evaluation of Adaptation Options for Key Marine Fisheries in Australia's South East</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Galappaththi, EK and Susarla, VB and Loutet, SJT and Ichien, ST and Hyman, AA and Ford, JD</t>
+          <t>Ogier, E and Jennings, S and Fowler, A and Frusher, S and Gardner, C and Hamer, P and Hobday, AJ and Linanne, A and Mayfield, S and Mundy, C and Sullivan, A and Tuck, G and Ward, T and Pecl, G</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>10.1111/faf.12595</t>
+          <t>10.3389/fmars.2020.00097</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Resilience and Social Adaptation to Climate Change Impacts in Small-Scale Fisheries</t>
+          <t>Fingerprinting Blue Carbon: Rationale and Tools to Determine the Source of Organic Carbon in Marine Depositional Environments</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Villasante, S and Macho, G and Silva, MRO and Lopes, PFM and Pita, P and Simon, A and Balsa, JCM and Olabarria, C and Vazquez, E and Calvo, N</t>
+          <t>Geraldi, NR and Ortega, A and Serrano, O and Macreadie, PI and Lovelock, CE and Krause-Jensen, D and Kennedy, H and Lavery, PS and Pace, ML and Kaal, J and Duarte, CM</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2022.802762</t>
+          <t>10.3389/fmars.2019.00263</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Responding to Climate Change: Participatory Evaluation of Adaptation Options for Key Marine Fisheries in Australia's South East</t>
+          <t>Key Challenges in Advancing an Ecosystem-Based Approach to Marine Spatial Planning Under Economic Growth Imperatives</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ogier, E and Jennings, S and Fowler, A and Frusher, S and Gardner, C and Hamer, P and Hobday, AJ and Linanne, A and Mayfield, S and Mundy, C and Sullivan, A and Tuck, G and Ward, T and Pecl, G</t>
+          <t>Lombard, AT and Dorrington, RA and Reed, JR and Ortega-Cisneros, K and Penry, GS and Pichegru, L and Smit, KP and Vermeulen, EA and Witteveen, M and Sink, KJ and Mcinnes, AM and Ginsburg, T</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2020.00097</t>
+          <t>10.3389/fmars.2019.00146</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Fingerprinting Blue Carbon: Rationale and Tools to Determine the Source of Organic Carbon in Marine Depositional Environments</t>
+          <t>Ocean Solutions to Address Climate Change and Its Effects on Marine Ecosystems</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Geraldi, NR and Ortega, A and Serrano, O and Macreadie, PI and Lovelock, CE and Krause-Jensen, D and Kennedy, H and Lavery, PS and Pace, ML and Kaal, J and Duarte, CM</t>
+          <t>Gattuso, JP and Magnan, AK and Bopp, L and Cheung, WWL and Duarte, CM and Hinkel, J and Mcleod, E and Micheli, F and Oschlies, A and Williamson, P and Bille, R and Chalastani, VI and Gates, RD and Irisson, JO and Middelburg, JJ and Portner, HO and Rau, GH</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2019.00263</t>
+          <t>10.3389/fmars.2018.00337</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Key Challenges in Advancing an Ecosystem-Based Approach to Marine Spatial Planning Under Economic Growth Imperatives</t>
+          <t>Limits on the adaptability of coastal marshes to rising sea level</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Lombard, AT and Dorrington, RA and Reed, JR and Ortega-Cisneros, K and Penry, GS and Pichegru, L and Smit, KP and Vermeulen, EA and Witteveen, M and Sink, KJ and Mcinnes, AM and Ginsburg, T</t>
+          <t>Kirwan, ML and Guntenspergen, GR and D'Alpaos, A and Morris, JT and Mudd, SM and Temmerman, S</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2019.00146</t>
+          <t>10.1029/2010GL045489</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Ocean Solutions to Address Climate Change and Its Effects on Marine Ecosystems</t>
+          <t>Climate engineering by artificial ocean upwelling: Channelling the sorcerer's apprentice</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Gattuso, JP and Magnan, AK and Bopp, L and Cheung, WWL and Duarte, CM and Hinkel, J and Mcleod, E and Micheli, F and Oschlies, A and Williamson, P and Bille, R and Chalastani, VI and Gates, RD and Irisson, JO and Middelburg, JJ and Portner, HO and Rau, GH</t>
+          <t>Oschlies, A and Pahlow, M and Yool, A and Matear, RJ</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2010</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>10.3389/fmars.2018.00337</t>
+          <t>10.1029/2009GL041961</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Limits on the adaptability of coastal marshes to rising sea level</t>
+          <t>Globalizing results from ocean in situ iron fertilization studies</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Kirwan, ML and Guntenspergen, GR and D'Alpaos, A and Morris, JT and Mudd, SM and Temmerman, S</t>
+          <t>Aumont, O and Bopp, L</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2006</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>10.1029/2010GL045489</t>
+          <t>10.1029/2005GB002591</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Climate engineering by artificial ocean upwelling: Channelling the sorcerer's apprentice</t>
+          <t>The impact of mobile demersal fishing on carbon storage in seabed sediments</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Oschlies, A and Pahlow, M and Yool, A and Matear, RJ</t>
+          <t>Epstein, G and Middelburg, JJ and Hawkins, JP and Norris, CR and Roberts, CM</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>2010</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>10.1029/2009GL041961</t>
+          <t>10.1111/gcb.16105</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Globalizing results from ocean in situ iron fertilization studies</t>
+          <t>Succession and seasonal dynamics of the epifauna community on offshore wind farm foundations and their role as stepping stones for non-indigenous species</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Aumont, O and Bopp, L</t>
+          <t>De Mesel, I and Kerckhof, F and Norro, A and Rumes, B and Degraer, S</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>2006</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>10.1029/2005GB002591</t>
+          <t>10.1007/s10750-014-2157-1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>The impact of mobile demersal fishing on carbon storage in seabed sediments</t>
+          <t>A review of adaptation options in fisheries management to support resilience and transition under socio-ecological change</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Epstein, G and Middelburg, JJ and Hawkins, JP and Norris, CR and Roberts, CM</t>
+          <t>Woods, PJ and Macdonald, JI and Bardarson, H and Bonanomi, S and Boonstra, WJ and Cornell, G and Cripps, G and Danielsen, R and Farber, L and Ferreira, ASA and Ferguson, K and Holma, M and Holt, RE and Hunter, KL and Kokkalis, A and Langbehn, TJ and Ljungstrom, G and Nieminen, E and Nordstrom, MC and Oostdijk, M and Richter, A and Romagnoni, G and Sguotti, C and Simons, A and Shackell, NL and Snickars, M and Whittington, JD and Wootton, H and Yletyinen, J</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1255,129 +1255,129 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>10.1111/gcb.16105</t>
+          <t>10.1093/icesjms/fsab146</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Succession and seasonal dynamics of the epifauna community on offshore wind farm foundations and their role as stepping stones for non-indigenous species</t>
+          <t>Responsive harvest control rules provide inherent resilience to adverse effects of climate change and scientific uncertainty</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>De Mesel, I and Kerckhof, F and Norro, A and Rumes, B and Degraer, S</t>
+          <t>Kritzer, JP and Costello, C and Mangin, T and Smith, SL</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>10.1007/s10750-014-2157-1</t>
+          <t>10.1093/icesjms/fsz038</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>A review of adaptation options in fisheries management to support resilience and transition under socio-ecological change</t>
+          <t>Greening of grey infrastructure should not be used as a Trojan horse to facilitate coastal development</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Woods, PJ and Macdonald, JI and Bardarson, H and Bonanomi, S and Boonstra, WJ and Cornell, G and Cripps, G and Danielsen, R and Farber, L and Ferreira, ASA and Ferguson, K and Holma, M and Holt, RE and Hunter, KL and Kokkalis, A and Langbehn, TJ and Ljungstrom, G and Nieminen, E and Nordstrom, MC and Oostdijk, M and Richter, A and Romagnoni, G and Sguotti, C and Simons, A and Shackell, NL and Snickars, M and Whittington, JD and Wootton, H and Yletyinen, J</t>
+          <t>Firth, LB and Airoldi, L and Bulleri, F and Challinor, S and Chee, SY and Evans, AJ and Hanley, ME and Knights, AM and O'Shaughnessy, K and Thompson, RC and Hawkins, SJ</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>10.1093/icesjms/fsab146</t>
+          <t>10.1111/1365-2664.13683</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Responsive harvest control rules provide inherent resilience to adverse effects of climate change and scientific uncertainty</t>
+          <t>Marine renewable energy: potential benefits to biodiversity? An urgent call for research</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Kritzer, JP and Costello, C and Mangin, T and Smith, SL</t>
+          <t>Inger, R and Attrill, MJ and Bearhop, S and Broderick, AC and Grecian, WJ and Hodgson, DJ and Mills, C and Sheehan, E and Votier, SC and Witt, MJ and Godley, BJ</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2009</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>10.1093/icesjms/fsz038</t>
+          <t>10.1111/j.1365-2664.2009.01697.x</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Greening of grey infrastructure should not be used as a Trojan horse to facilitate coastal development</t>
+          <t>Eco-efficiency assessment of wave energy conversion in Western Australia</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Firth, LB and Airoldi, L and Bulleri, F and Challinor, S and Chee, SY and Evans, AJ and Hanley, ME and Knights, AM and O'Shaughnessy, K and Thompson, RC and Hawkins, SJ</t>
+          <t>Burgess, C and Biswas, WK</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>10.1111/1365-2664.13683</t>
+          <t>10.1016/j.jclepro.2021.127814</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Marine renewable energy: potential benefits to biodiversity? An urgent call for research</t>
+          <t>Land raising as a solution to sea-level rise: An analysis of coastal flooding on an artificial island in the Maldives</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Inger, R and Attrill, MJ and Bearhop, S and Broderick, AC and Grecian, WJ and Hodgson, DJ and Mills, C and Sheehan, E and Votier, SC and Witt, MJ and Godley, BJ</t>
+          <t>Brown, S and Wadey, MP and Nicholls, RJ and Shareef, A and Khaleel, Z and Hinkel, J and Lincke, D and McCabe, MV</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>2009</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>10.1111/j.1365-2664.2009.01697.x</t>
+          <t>10.1111/jfr3.12567</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Eco-efficiency assessment of wave energy conversion in Western Australia</t>
+          <t>Tidal and Nontidal Marsh Restoration: A Trade-Off Between Carbon Sequestration, Methane Emissions, and Soil Accretion</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Burgess, C and Biswas, WK</t>
+          <t>Arias-Ortiz, A and Oikawa, PY and Carlin, J and Masque, P and Shahan, J and Kanneg, S and Paytan, A and Baldocchi, DD</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1387,41 +1387,41 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>10.1016/j.jclepro.2021.127814</t>
+          <t>10.1029/2021JG006573</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Land raising as a solution to sea-level rise: An analysis of coastal flooding on an artificial island in the Maldives</t>
+          <t>Constraining Marsh Carbon Budgets Using Long-Term C Burial and Contemporary Atmospheric CO2 Fluxes</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Brown, S and Wadey, MP and Nicholls, RJ and Shareef, A and Khaleel, Z and Hinkel, J and Lincke, D and McCabe, MV</t>
+          <t>Forbrich, I and Giblin, AE and Hopkinson, CS</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>10.1111/jfr3.12567</t>
+          <t>10.1002/2017JG004336</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Tidal and Nontidal Marsh Restoration: A Trade-Off Between Carbon Sequestration, Methane Emissions, and Soil Accretion</t>
+          <t>A review of tidal energy-Resource, feedbacks, and environmental interactions</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Arias-Ortiz, A and Oikawa, PY and Carlin, J and Masque, P and Shahan, J and Kanneg, S and Paytan, A and Baldocchi, DD</t>
+          <t>Neill, SP and Haas, KA and Thiebot, J and Yang, ZQ</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1431,987 +1431,987 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>10.1029/2021JG006573</t>
+          <t>10.1063/5.0069452</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Constraining Marsh Carbon Budgets Using Long-Term C Burial and Contemporary Atmospheric CO2 Fluxes</t>
+          <t>Organic carbon dynamics and microbial community response to oyster reef restoration</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Forbrich, I and Giblin, AE and Hopkinson, CS</t>
+          <t>Hurst, NR and Locher, B and Steinmuller, HE and Walters, LJ and Chambers, LG</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>10.1002/2017JG004336</t>
+          <t>10.1002/lno.12063</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>A review of tidal energy-Resource, feedbacks, and environmental interactions</t>
+          <t>Can macroalgae contribute to blue carbon? An Australian perspective</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Neill, SP and Haas, KA and Thiebot, J and Yang, ZQ</t>
+          <t>Hill, R and Bellgrove, A and Macreadie, PI and Petrou, K and Beardall, J and Steven, A and Ralph, PJ</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>10.1063/5.0069452</t>
+          <t>10.1002/lno.10128</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Organic carbon dynamics and microbial community response to oyster reef restoration</t>
+          <t>Low genetic connectivity in a fouling amphipod among man-made structures in the southern North Sea</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Hurst, NR and Locher, B and Steinmuller, HE and Walters, LJ and Chambers, LG</t>
+          <t>Luttikhuizen, PC and Beermann, J and Crooijmans, RPMA and Jak, RG and Coolen, JWP</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>10.1002/lno.12063</t>
+          <t>10.3354/meps12929</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Can macroalgae contribute to blue carbon? An Australian perspective</t>
+          <t>Leveraging new knowledge of Symbiodinium community regulation in corals for conservation and reef restoration</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Hill, R and Bellgrove, A and Macreadie, PI and Petrou, K and Beardall, J and Steven, A and Ralph, PJ</t>
+          <t>Quigley, KM and Bay, LK and Willis, BL</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>10.1002/lno.10128</t>
+          <t>10.3354/meps12652</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Low genetic connectivity in a fouling amphipod among man-made structures in the southern North Sea</t>
+          <t>Windfarms, fishing and benthic recovery: Overlaps, risks and opportunities</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Luttikhuizen, PC and Beermann, J and Crooijmans, RPMA and Jak, RG and Coolen, JWP</t>
+          <t>Dunkley, F and Solandt, JL</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>10.3354/meps12929</t>
+          <t>10.1016/j.marpol.2022.105262</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Leveraging new knowledge of Symbiodinium community regulation in corals for conservation and reef restoration</t>
+          <t>Implementation of blue carbon offset crediting for seagrass meadows, macroalgal beds, and macroalgae farming in Japan</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Quigley, KM and Bay, LK and Willis, BL</t>
+          <t>Kuwae, T and Watanabe, A and Yoshihara, S and Suehiro, F and Sugimura, Y</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>10.3354/meps12652</t>
+          <t>10.1016/j.marpol.2022.104996</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Windfarms, fishing and benthic recovery: Overlaps, risks and opportunities</t>
+          <t>Genome-wide SNP analysis reveals an increase in adaptive genetic variation through selective breeding of coral</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Dunkley, F and Solandt, JL</t>
+          <t>Quigley, KM and Bay, LK and van Oppen, MJH</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>10.1016/j.marpol.2022.105262</t>
+          <t>10.1111/mec.15482</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Implementation of blue carbon offset crediting for seagrass meadows, macroalgal beds, and macroalgae farming in Japan</t>
+          <t>Marine stepping-stones: Connectivity of Mytilus edulis populations between offshore energy installations</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Kuwae, T and Watanabe, A and Yoshihara, S and Suehiro, F and Sugimura, Y</t>
+          <t>Coolen, JWP and Boon, AR and Crooijmans, R and van Pelt, H and Kleissen, F and Gerla, D and Beermann, J and Birchenough, SNR and Becking, LE and Luttikhuizen, PC</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>10.1016/j.marpol.2022.104996</t>
+          <t>10.1111/mec.15364</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Genome-wide SNP analysis reveals an increase in adaptive genetic variation through selective breeding of coral</t>
+          <t>Reversal of ocean acidification enhances net coral reef calcification</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Quigley, KM and Bay, LK and van Oppen, MJH</t>
+          <t>Albright, R and Caldeira, L and Hosfelt, J and Kwiatkowski, L and Maclaren, JK and Mason, BM and Nebuchina, Y and Ninokawa, A and Pongratz, J and Ricke, KL and Rivlin, T and Schneider, K and Sesboue, M and Shamberger, K and Silverman, J and Wolfe, K and Zhu, K and Caldeira, K</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>10.1111/mec.15482</t>
+          <t>10.1038/nature17155</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Marine stepping-stones: Connectivity of Mytilus edulis populations between offshore energy installations</t>
+          <t>Building adaptive capacity to climate change in tropical coastal communities</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Coolen, JWP and Boon, AR and Crooijmans, R and van Pelt, H and Kleissen, F and Gerla, D and Beermann, J and Birchenough, SNR and Becking, LE and Luttikhuizen, PC</t>
+          <t>Cinner, JE and Adger, WN and Allison, EH and Barnes, ML and Brown, K and Cohen, PJ and Gelcich, S and Hicks, CC and Hughes, TP and Lau, J and Marshall, NA and Morrison, TH</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>10.1111/mec.15364</t>
+          <t>10.1038/s41558-017-0065-x</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Reversal of ocean acidification enhances net coral reef calcification</t>
+          <t>Testing the climate intervention potential of ocean afforestation using the Great Atlantic Sargassum Belt</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Albright, R and Caldeira, L and Hosfelt, J and Kwiatkowski, L and Maclaren, JK and Mason, BM and Nebuchina, Y and Ninokawa, A and Pongratz, J and Ricke, KL and Rivlin, T and Schneider, K and Sesboue, M and Shamberger, K and Silverman, J and Wolfe, K and Zhu, K and Caldeira, K</t>
+          <t>Bach, LT and Tamsitt, V and Gower, J and Hurd, CL and Raven, JA and Boyd, PW</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>10.1038/nature17155</t>
+          <t>10.1038/s41467-021-22837-2</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Building adaptive capacity to climate change in tropical coastal communities</t>
+          <t>Australian vegetated coastal ecosystems as global hotspots for climate change mitigation</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Cinner, JE and Adger, WN and Allison, EH and Barnes, ML and Brown, K and Cohen, PJ and Gelcich, S and Hicks, CC and Hughes, TP and Lau, J and Marshall, NA and Morrison, TH</t>
+          <t>Serrano, O and Lovelock, CE and Atwood, TB and Macreadie, PI and Canto, R and Phinn, S and Arias-Ortiz, A and Bai, L and Baldock, J and Bedulli, C and Carnell, P and Connolly, RM and Donaldson, P and Esteban, A and Lewis, CJE and Eyre, BD and Hayes, MA and Horwitz, P and Hutley, LB and Kavazos, CRJ and Kelleway, JJ and Kendrick, GA and Kilminster, K and Lafratta, A and Lee, S and Lavery, PS and Maher, DT and Marba, N and Masque, P and Mateo, MA and Mount, R and Ralph, PJ and Roelfsema, C and Rozaimi, M and Ruhon, R and Salinas, C and Samper-Villarreal, J and Sanderman, J and Sanders, CJ and Santos, I and Sharples, C and Steven, ADL and Cannard, T and Trevathan-Tackett, SM and Duarte, CM</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>10.1038/s41558-017-0065-x</t>
+          <t>10.1038/s41467-019-12176-8</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Harnessing nature to help people adapt to climate change</t>
+          <t>Potential climate engineering effectiveness and side effects during a high carbon dioxide-emission scenario</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Jones, HP and Hole, DG and Zavaleta, ES</t>
+          <t>Keller, DP and Feng, EY and Oschlies, A</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>2012</t>
+          <t>2014</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>10.1038/NCLIMATE1463</t>
+          <t>10.1038/ncomms4304</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Testing the climate intervention potential of ocean afforestation using the Great Atlantic Sargassum Belt</t>
+          <t>Potential negative effects of ocean afforestation on offshore ecosystems</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Bach, LT and Tamsitt, V and Gower, J and Hurd, CL and Raven, JA and Boyd, PW</t>
+          <t>Boyd, PW and Bach, LT and Hurd, CL and Paine, E and Raven, JA and Tamsitt, V</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>10.1038/s41467-021-22837-2</t>
+          <t>10.1038/s41559-022-01722-1</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Australian vegetated coastal ecosystems as global hotspots for climate change mitigation</t>
+          <t>Potential use of engineered nanoparticles in ocean fertilization for large-scale atmospheric carbon dioxide removal</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Serrano, O and Lovelock, CE and Atwood, TB and Macreadie, PI and Canto, R and Phinn, S and Arias-Ortiz, A and Bai, L and Baldock, J and Bedulli, C and Carnell, P and Connolly, RM and Donaldson, P and Esteban, A and Lewis, CJE and Eyre, BD and Hayes, MA and Horwitz, P and Hutley, LB and Kavazos, CRJ and Kelleway, JJ and Kendrick, GA and Kilminster, K and Lafratta, A and Lee, S and Lavery, PS and Maher, DT and Marba, N and Masque, P and Mateo, MA and Mount, R and Ralph, PJ and Roelfsema, C and Rozaimi, M and Ruhon, R and Salinas, C and Samper-Villarreal, J and Sanderman, J and Sanders, CJ and Santos, I and Sharples, C and Steven, ADL and Cannard, T and Trevathan-Tackett, SM and Duarte, CM</t>
+          <t>Babakhani, P and Phenrat, T and Baalousha, M and Soratana, K and Peacock, CL and Twining, BS and Hochella, MF</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>10.1038/s41467-019-12176-8</t>
+          <t>10.1038/s41565-022-01226-w</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Potential climate engineering effectiveness and side effects during a high carbon dioxide-emission scenario</t>
+          <t>Blue carbon as a natural climate solution</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Keller, DP and Feng, EY and Oschlies, A</t>
+          <t>Macreadie, PI and Costa, MDP and Atwood, TB and Friess, DA and Kelleway, JJ and Kennedy, H and Lovelock, CE and Serrano, O and Duarte, CM</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>2014</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>10.1038/ncomms4304</t>
+          <t>10.1038/s43017-021-00224-1</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Potential negative effects of ocean afforestation on offshore ecosystems</t>
+          <t>Extending the natural adaptive capacity of coral holobionts</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Boyd, PW and Bach, LT and Hurd, CL and Paine, E and Raven, JA and Tamsitt, V</t>
+          <t>Voolstra, CR and Suggett, DJ and Peixoto, RS and Parkinson, JE and Quigley, KM and Silveira, CB and Sweet, M and Muller, EM and Barshis, DJ and Bourne, DG and Aranda, M</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>10.1038/s41559-022-01722-1</t>
+          <t>10.1038/s43017-021-00214-3</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Potential use of engineered nanoparticles in ocean fertilization for large-scale atmospheric carbon dioxide removal</t>
+          <t>Coastal residents' perceptions of the function of and relationship between engineered and natural infrastructure for coastal hazard mitigation</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Babakhani, P and Phenrat, T and Baalousha, M and Soratana, K and Peacock, CL and Twining, BS and Hochella, MF</t>
+          <t>Gray, JDE and O'Neill, K and Qiu, ZY</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>10.1038/s41565-022-01226-w</t>
+          <t>10.1016/j.ocecoaman.2017.07.005</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Blue carbon as a natural climate solution</t>
+          <t>Swansea Bay tidal lagoon annual energy estimation</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Macreadie, PI and Costa, MDP and Atwood, TB and Friess, DA and Kelleway, JJ and Kennedy, H and Lovelock, CE and Serrano, O and Duarte, CM</t>
+          <t>Petley, S and Aggidis, G</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2016</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>10.1038/s43017-021-00224-1</t>
+          <t>10.1016/j.oceaneng.2015.11.022</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Extending the natural adaptive capacity of coral holobionts</t>
+          <t>Sustainable artificial island concept for the Republic of Kiribati</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Voolstra, CR and Suggett, DJ and Peixoto, RS and Parkinson, JE and Quigley, KM and Silveira, CB and Sweet, M and Muller, EM and Barshis, DJ and Bourne, DG and Aranda, M</t>
+          <t>Lister, N and Muk-Pavic, E</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2015</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>10.1038/s43017-021-00214-3</t>
+          <t>10.1016/j.oceaneng.2015.01.013</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Coastal residents' perceptions of the function of and relationship between engineered and natural infrastructure for coastal hazard mitigation</t>
+          <t>Ocean conservation boosts climate change mitigation and adaptation</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Gray, JDE and O'Neill, K and Qiu, ZY</t>
+          <t>Jacquemont, J and Blasiak, R and Le Cam, C and Le Gouellec, M and Claudet, J</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>10.1016/j.ocecoaman.2017.07.005</t>
+          <t>10.1016/j.oneear.2022.09.002</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Swansea Bay tidal lagoon annual energy estimation</t>
+          <t>Operationalizing marketable blue carbon</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Petley, S and Aggidis, G</t>
+          <t>Macreadie, PI and Robertson, AI and Spinks, B and Adams, MP and Atchison, JM and Bell-James, J and Bryan, BA and Chu, L and Filbee-Dexter, K and Drake, L and Duarte, CM and Friess, DA and Gonzalez, F and Grafton, RQ and Helmstedt, KJ and Kaebernick, M and Kelleway, J and Kendrick, GA and Kennedy, H and Lovelock, CE and Megonigal, JP and Maher, DT and Pidgeon, E and Rogers, AA and Sturgiss, R and Trevathan-Tackett, SM and Wartman, M and Wilson, KA and Rogers, K</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>2016</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>10.1016/j.oceaneng.2015.11.022</t>
+          <t>10.1016/j.oneear.2022.04.005</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Sustainable artificial island concept for the Republic of Kiribati</t>
+          <t>Realistic fisheries management reforms could mitigate the impacts of climate change in most countries</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Lister, N and Muk-Pavic, E</t>
+          <t>Free, CM and Mangin, T and Molinos, JG and Ojea, E and Burden, M and Costello, C and Gaines, SD</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>2015</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>10.1016/j.oceaneng.2015.01.013</t>
+          <t>10.1371/journal.pone.0224347</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Ocean conservation boosts climate change mitigation and adaptation</t>
+          <t>Using naturally occurring climate resilient corals to construct bleaching-resistant nurseries</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Jacquemont, J and Blasiak, R and Le Cam, C and Le Gouellec, M and Claudet, J</t>
+          <t>Morikawa, MK and Palumbi, SR</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>10.1016/j.oneear.2022.09.002</t>
+          <t>10.1073/pnas.1721415116</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Operationalizing marketable blue carbon</t>
+          <t>Marine reserves can mitigate and promote adaptation to climate change</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Macreadie, PI and Robertson, AI and Spinks, B and Adams, MP and Atchison, JM and Bell-James, J and Bryan, BA and Chu, L and Filbee-Dexter, K and Drake, L and Duarte, CM and Friess, DA and Gonzalez, F and Grafton, RQ and Helmstedt, KJ and Kaebernick, M and Kelleway, J and Kendrick, GA and Kennedy, H and Lovelock, CE and Megonigal, JP and Maher, DT and Pidgeon, E and Rogers, AA and Sturgiss, R and Trevathan-Tackett, SM and Wartman, M and Wilson, KA and Rogers, K</t>
+          <t>Roberts, CM and O'Leary, BC and McCauley, DJ and Cury, PM and Duarte, CM and Lubchenco, J and Pauly, D and Saenz-Arroyo, A and Sumaila, UR and Wilson, RW and Worm, B and Castilla, JC</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>10.1016/j.oneear.2022.04.005</t>
+          <t>10.1073/pnas.1701262114</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Realistic fisheries management reforms could mitigate the impacts of climate change in most countries</t>
+          <t>Climate change damages to Alaska public infrastructure and the economics of proactive adaptation</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Free, CM and Mangin, T and Molinos, JG and Ojea, E and Burden, M and Costello, C and Gaines, SD</t>
+          <t>Melvin, AM and Larsen, P and Boehlert, B and Neumann, JE and Chinowsky, P and Espinet, X and Martinich, J and Baumann, MS and Rennels, L and Bothner, A and Nicolsky, DJ and Marchenko, SS</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2017</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>10.1371/journal.pone.0224347</t>
+          <t>10.1073/pnas.1611056113</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Using naturally occurring climate resilient corals to construct bleaching-resistant nurseries</t>
+          <t>Towards adaptation pathways for atoll islands. Insights from the Maldives</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Morikawa, MK and Palumbi, SR</t>
+          <t>Magnan, AK and Duvat, VKE</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>10.1073/pnas.1721415116</t>
+          <t>10.1007/s10113-020-01691-w</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Marine reserves can mitigate and promote adaptation to climate change</t>
+          <t>Assessment of coastal risk reduction and adaptation-labelled responses in Mauritius Island (Indian Ocean)</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Roberts, CM and O'Leary, BC and McCauley, DJ and Cury, PM and Duarte, CM and Lubchenco, J and Pauly, D and Saenz-Arroyo, A and Sumaila, UR and Wilson, RW and Worm, B and Castilla, JC</t>
+          <t>Duvat, VKE and Anisimov, A and Magnan, AK</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>10.1073/pnas.1701262114</t>
+          <t>10.1007/s10113-020-01699-2</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Climate change damages to Alaska public infrastructure and the economics of proactive adaptation</t>
+          <t>Heading for the hills: climate-driven community relocations in the Solomon Islands and Alaska provide insight for a 1.5 degrees C future</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Melvin, AM and Larsen, P and Boehlert, B and Neumann, JE and Chinowsky, P and Espinet, X and Martinich, J and Baumann, MS and Rennels, L and Bothner, A and Nicolsky, DJ and Marchenko, SS</t>
+          <t>Albert, S and Bronen, R and Tooler, N and Leon, J and Yee, D and Ash, J and Boseto, D and Grinham, A</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>2017</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>10.1073/pnas.1611056113</t>
+          <t>10.1007/s10113-017-1256-8</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Towards adaptation pathways for atoll islands. Insights from the Maldives</t>
+          <t>Quantifying the effects of tidal turbine array operations on the distribution of marine mammals: Implications for collision risk</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Magnan, AK and Duvat, VKE</t>
+          <t>Onoufriou, J and Russell, DJF and Thompson, D and Moss, SE and Hastie, GD</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>10.1007/s10113-020-01691-w</t>
+          <t>10.1016/j.renene.2021.08.052</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Assessment of coastal risk reduction and adaptation-labelled responses in Mauritius Island (Indian Ocean)</t>
+          <t>Six priorities to advance the science and practice of coral reef restoration worldwide</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Duvat, VKE and Anisimov, A and Magnan, AK</t>
+          <t>Vardi, T and Hoot, WC and Levy, J and Shaver, E and Winters, RS and Banaszak, AT and Baums, IB and Chamberland, V and Cook, N and Gulko, D and Hein, MY and Kaufman, L and Loewe, M and Lundgren, P and Lustic, C and MacGowan, P and Matz, MV and McGonigle, M and McLeod, I and Moore, J and Moore, T and Pivard, S and Pollock, FJ and Rinkevich, B and Suggett, DJ and Suleiman, S and Viehman, TS and Villalobos, T and Weis, VM and Wolke, C and MontoyaMaya, PH</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>10.1007/s10113-020-01699-2</t>
+          <t>10.1111/rec.13498</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Heading for the hills: climate-driven community relocations in the Solomon Islands and Alaska provide insight for a 1.5 degrees C future</t>
+          <t>Symbiodiniaceae probiotics for use in bleaching recovery</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Albert, S and Bronen, R and Tooler, N and Leon, J and Yee, D and Ash, J and Boseto, D and Grinham, A</t>
+          <t>Morgans, CA and Hung, JY and Bourne, DG and Quigley, KM</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>10.1007/s10113-017-1256-8</t>
+          <t>10.1111/rec.13069</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Quantifying the effects of tidal turbine array operations on the distribution of marine mammals: Implications for collision risk</t>
+          <t>The potential for created oyster shell reefs as a sustainable shoreline protection strategy in Louisiana</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Onoufriou, J and Russell, DJF and Thompson, D and Moss, SE and Hastie, GD</t>
+          <t>Piazza, BP and Banks, PD and La Peyre, MK</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2005</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>10.1016/j.renene.2021.08.052</t>
+          <t>10.1111/j.1526-100X.2005.00062.x</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Six priorities to advance the science and practice of coral reef restoration worldwide</t>
+          <t>Direct experiments on the ocean disposal of fossil fuel CO2</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Vardi, T and Hoot, WC and Levy, J and Shaver, E and Winters, RS and Banaszak, AT and Baums, IB and Chamberland, V and Cook, N and Gulko, D and Hein, MY and Kaufman, L and Loewe, M and Lundgren, P and Lustic, C and MacGowan, P and Matz, MV and McGonigle, M and McLeod, I and Moore, J and Moore, T and Pivard, S and Pollock, FJ and Rinkevich, B and Suggett, DJ and Suleiman, S and Viehman, TS and Villalobos, T and Weis, VM and Wolke, C and MontoyaMaya, PH</t>
+          <t>Brewer, PG and Friederich, C and Peltzer, ET and Orr, FM</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>1999</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>10.1111/rec.13498</t>
+          <t>10.1126/science.284.5416.943</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Symbiodiniaceae probiotics for use in bleaching recovery</t>
+          <t>Coral microbiome manipulation elicits metabolic and genetic restructuring to mitigate heat stress and evade mortality</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Morgans, CA and Hung, JY and Bourne, DG and Quigley, KM</t>
+          <t>Santoro, EP and Borges, RM and Espinoza, JL and Freire, M and Messias, CSMA and Villela, HDM and Pereira, LM and Vilela, CLS and Rosado, JG and Cardoso, PM and Rosado, PM and Assis, JM and Duarte, GAS and Perna, G and Rosado, AS and Macrae, A and Dupont, CL and Nelson, KE and Sweet, MJ and Voolstra, CR and Peixoto, RS</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2021</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>10.1111/rec.13069</t>
+          <t>10.1126/sciadv.abg3088</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>The potential for created oyster shell reefs as a sustainable shoreline protection strategy in Louisiana</t>
+          <t>Heat-evolved microalgal symbionts increase coral bleaching tolerance</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Piazza, BP and Banks, PD and La Peyre, MK</t>
+          <t>Buerger, P and Alvarez-Roa, C and Coppin, CW and Pearce, SL and Chakravarti, LJ and Oakeshott, JG and Edwards, R and van Oppen, MJH</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>2005</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>10.1111/j.1526-100X.2005.00062.x</t>
+          <t>10.1126/sciadv.aba2498</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Direct experiments on the ocean disposal of fossil fuel CO2</t>
+          <t>Managed retreat through voluntary buyouts of flood-prone properties</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Brewer, PG and Friederich, C and Peltzer, ET and Orr, FM</t>
+          <t>Mach, KJ and Kraan, CM and Hino, M and Siders, AR and Johnston, EM and Field, CB</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>1999</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>10.1126/science.284.5416.943</t>
+          <t>10.1126/sciadv.aax8995</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Coral microbiome manipulation elicits metabolic and genetic restructuring to mitigate heat stress and evade mortality</t>
+          <t>Improved fisheries management could offset many negative effects of climate change</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Santoro, EP and Borges, RM and Espinoza, JL and Freire, M and Messias, CSMA and Villela, HDM and Pereira, LM and Vilela, CLS and Rosado, JG and Cardoso, PM and Rosado, PM and Assis, JM and Duarte, GAS and Perna, G and Rosado, AS and Macrae, A and Dupont, CL and Nelson, KE and Sweet, MJ and Voolstra, CR and Peixoto, RS</t>
+          <t>Gaines, SD and Costello, C and Owashi, B and Mangin, T and Bone, J and Molinos, JG and Burden, M and Dennis, H and Halpern, BS and Kappel, CV and Kleisner, KM and Ovando, D</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>2021</t>
+          <t>2018</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.abg3088</t>
+          <t>10.1126/sciadv.aao1378</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Heat-evolved microalgal symbionts increase coral bleaching tolerance</t>
+          <t>Unravelling the ecological impacts of large-scale offshore wind farms in the Mediterranean Sea</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Buerger, P and Alvarez-Roa, C and Coppin, CW and Pearce, SL and Chakravarti, LJ and Oakeshott, JG and Edwards, R and van Oppen, MJH</t>
+          <t>Lloret, J and Turiel, A and Sole, J and Berdalet, E and Sabates, A and Olivares, A and Gili, JM and Vila-Subiros, J and Sarda, R</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.aba2498</t>
+          <t>10.1016/j.scitotenv.2022.153803</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Managed retreat through voluntary buyouts of flood-prone properties</t>
+          <t>Climate adaptation pathways and the role of social-ecological networks in small-scale fisheries</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Mach, KJ and Kraan, CM and Hino, M and Siders, AR and Johnston, EM and Field, CB</t>
+          <t>Salgueiro-Otero, D and Barnes, ML and Ojea, E</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>2019</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.aax8995</t>
+          <t>10.1038/s41598-022-18668-w</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Improved fisheries management could offset many negative effects of climate change</t>
+          <t>Internal relocation as a relevant and feasible adaptation strategy in Rangiroa Atoll, French Polynesia</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Gaines, SD and Costello, C and Owashi, B and Mangin, T and Bone, J and Molinos, JG and Burden, M and Dennis, H and Halpern, BS and Kappel, CV and Kleisner, KM and Ovando, D</t>
+          <t>Duvat, VKE and Magnan, AK and Goeldner-Gianella, L and Grancher, D and Costa, S and Maquaire, O and Le Cozannet, G and Stahl, L and Volto, N and Pignon-Mussaud, C</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>2018</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>10.1126/sciadv.aao1378</t>
+          <t>10.1038/s41598-022-18109-8</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Unravelling the ecological impacts of large-scale offshore wind farms in the Mediterranean Sea</t>
+          <t>Marine protected areas do not prevent marine heatwave-induced fish community structure changes in a temperate transition zone</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Lloret, J and Turiel, A and Sole, J and Berdalet, E and Sabates, A and Olivares, A and Gili, JM and Vila-Subiros, J and Sarda, R</t>
+          <t>Freedman, RM and Brown, JA and Caldow, C and Caselle, JE</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>10.1016/j.scitotenv.2022.153803</t>
+          <t>10.1038/s41598-020-77885-3</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Climate adaptation pathways and the role of social-ecological networks in small-scale fisheries</t>
+          <t>Substantial blue carbon in overlooked Australian kelp forests</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Salgueiro-Otero, D and Barnes, ML and Ojea, E</t>
+          <t>Filbee-Dexter, K and Wernberg, T</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2020</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>10.1038/s41598-022-18668-w</t>
+          <t>10.1038/s41598-020-69258-7</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Internal relocation as a relevant and feasible adaptation strategy in Rangiroa Atoll, French Polynesia</t>
+          <t>Oyster breakwater reefs promote adjacent mudflat stability and salt marsh growth in a monsoon dominated subtropical coast</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Duvat, VKE and Magnan, AK and Goeldner-Gianella, L and Grancher, D and Costa, S and Maquaire, O and Le Cozannet, G and Stahl, L and Volto, N and Pignon-Mussaud, C</t>
+          <t>Chowdhury, MSN and Walles, B and Sharifuzzaman, SM and Hossain, MS and Ysebaert, T and Smaal, AC</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>2022</t>
+          <t>2019</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>10.1038/s41598-022-18109-8</t>
+          <t>10.1038/s41598-019-44925-6</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Marine protected areas do not prevent marine heatwave-induced fish community structure changes in a temperate transition zone</t>
+          <t>Taking control of human-induced destabilisation of atoll islands: lessons learnt from the Tuamotu Archipelago, French Polynesia</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Freedman, RM and Brown, JA and Caldow, C and Caselle, JE</t>
+          <t>Duvat, VKE and Stahl, L and Costa, S and Maquaire, O and Magnan, AK</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2421,93 +2421,27 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>10.1038/s41598-020-77885-3</t>
+          <t>10.1007/s11625-019-00722-8</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Substantial blue carbon in overlooked Australian kelp forests</t>
+          <t>Artificial hard-substrate colonisation in the offshore Nywind Scotland Pilot Park</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Filbee-Dexter, K and Wernberg, T</t>
+          <t>Karlsson, R and Tivefalth, M and Duranovic, I and Martinsson, S and Kjolhamar, A and Murvoll, KM</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>2020</t>
+          <t>2022</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
-        <is>
-          <t>10.1038/s41598-020-69258-7</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>Oyster breakwater reefs promote adjacent mudflat stability and salt marsh growth in a monsoon dominated subtropical coast</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Chowdhury, MSN and Walles, B and Sharifuzzaman, SM and Hossain, MS and Ysebaert, T and Smaal, AC</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>2019</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>10.1038/s41598-019-44925-6</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>Taking control of human-induced destabilisation of atoll islands: lessons learnt from the Tuamotu Archipelago, French Polynesia</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Duvat, VKE and Stahl, L and Costa, S and Maquaire, O and Magnan, AK</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>2020</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>10.1007/s11625-019-00722-8</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>Artificial hard-substrate colonisation in the offshore Nywind Scotland Pilot Park</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Karlsson, R and Tivefalth, M and Duranovic, I and Martinsson, S and Kjolhamar, A and Murvoll, KM</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>2022</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
         <is>
           <t>10.5194/wes-7-801-2022</t>
         </is>

</xml_diff>